<commit_message>
more updates on cht hts workflows and validations
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_initial_test.xlsx
+++ b/config/default/forms/app/hts_initial_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="413">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -312,7 +312,10 @@
     <t xml:space="preserve">selected(${_164401_everTestedByProvider_99DCT},'_1065_yes_99DCT')</t>
   </si>
   <si>
-    <t xml:space="preserve">.&gt;=0 and .&lt;=12</t>
+    <t xml:space="preserve">.&gt;=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accepts values above 0</t>
   </si>
   <si>
     <t xml:space="preserve">_164952_HasClientdoneHIVselfTestInlast12months_99DCT</t>
@@ -5729,28 +5732,26 @@
   </sheetPr>
   <dimension ref="A1:Y65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="112" zoomScaleNormal="112" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="I106" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
-      <selection pane="topRight" activeCell="A132" activeCellId="0" sqref="A132"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="112" zoomScaleNormal="112" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="H37" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+      <selection pane="topRight" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.0051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="87.2040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="71.0969387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.8469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="135.709183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="45.5357142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="54.4489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.5357142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.4081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.8979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="90.3520408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9897959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="73.6173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.9183673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="140.663265306122"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="47.1581632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="44.7295918367347"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="56.4285714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7157,7 +7158,7 @@
       <c r="X43" s="5"/>
       <c r="Y43" s="5"/>
     </row>
-    <row r="44" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
         <v>92</v>
       </c>
@@ -7175,7 +7176,9 @@
       <c r="G44" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H44" s="5"/>
+      <c r="H44" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
@@ -7199,10 +7202,10 @@
         <v>80</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>60</v>
@@ -7231,13 +7234,13 @@
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>60</v>
@@ -7269,16 +7272,16 @@
         <v>71</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="4"/>
@@ -7303,13 +7306,13 @@
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>60</v>
@@ -7341,16 +7344,16 @@
         <v>71</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>74</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="4"/>
@@ -7378,10 +7381,10 @@
         <v>80</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>60</v>
@@ -7410,19 +7413,19 @@
     </row>
     <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
@@ -7477,14 +7480,14 @@
         <v>13</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
@@ -7509,13 +7512,13 @@
     </row>
     <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>60</v>
@@ -7547,10 +7550,10 @@
         <v>71</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>60</v>
@@ -7582,10 +7585,10 @@
         <v>57</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>60</v>
@@ -7593,10 +7596,10 @@
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
@@ -7618,13 +7621,13 @@
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>60</v>
@@ -7653,19 +7656,19 @@
     </row>
     <row r="58" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
@@ -7722,14 +7725,14 @@
         <v>13</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
@@ -7754,17 +7757,17 @@
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
@@ -7792,14 +7795,14 @@
         <v>71</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
@@ -7827,21 +7830,21 @@
         <v>57</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F63" s="5"/>
       <c r="G63" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
@@ -7863,17 +7866,17 @@
     </row>
     <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
@@ -7930,7 +7933,7 @@
         <v>44</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -7939,7 +7942,7 @@
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J66" s="5"/>
       <c r="K66" s="5"/>
@@ -7963,7 +7966,7 @@
         <v>44</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -7972,7 +7975,7 @@
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="5"/>
@@ -7993,17 +7996,17 @@
     </row>
     <row r="68" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
@@ -8031,16 +8034,16 @@
         <v>80</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
@@ -8065,19 +8068,19 @@
     </row>
     <row r="70" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -8102,19 +8105,19 @@
     </row>
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>60</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
@@ -8142,10 +8145,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -8204,15 +8207,15 @@
         <v>13</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
@@ -8236,13 +8239,13 @@
     </row>
     <row r="75" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
@@ -8269,18 +8272,18 @@
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
@@ -8304,13 +8307,13 @@
     </row>
     <row r="77" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
@@ -8337,18 +8340,18 @@
     </row>
     <row r="78" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
@@ -8372,13 +8375,13 @@
     </row>
     <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -8405,20 +8408,20 @@
     </row>
     <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
@@ -8442,20 +8445,20 @@
     </row>
     <row r="81" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
@@ -8479,20 +8482,20 @@
     </row>
     <row r="82" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
@@ -8516,13 +8519,13 @@
     </row>
     <row r="83" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
@@ -8549,20 +8552,20 @@
     </row>
     <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
@@ -8586,20 +8589,20 @@
     </row>
     <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
@@ -8623,20 +8626,20 @@
     </row>
     <row r="86" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
@@ -8660,20 +8663,20 @@
     </row>
     <row r="87" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
@@ -8697,20 +8700,20 @@
     </row>
     <row r="88" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
@@ -8734,20 +8737,20 @@
     </row>
     <row r="89" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
@@ -8771,20 +8774,20 @@
     </row>
     <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
@@ -8808,20 +8811,20 @@
     </row>
     <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
@@ -8845,13 +8848,13 @@
     </row>
     <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -8878,20 +8881,20 @@
     </row>
     <row r="93" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F93" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -8915,20 +8918,20 @@
     </row>
     <row r="94" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F94" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
@@ -8952,20 +8955,20 @@
     </row>
     <row r="95" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
@@ -8989,20 +8992,20 @@
     </row>
     <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F96" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
@@ -9026,20 +9029,20 @@
     </row>
     <row r="97" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
@@ -9063,20 +9066,20 @@
     </row>
     <row r="98" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F98" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
@@ -9100,20 +9103,20 @@
     </row>
     <row r="99" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
@@ -9137,20 +9140,20 @@
     </row>
     <row r="100" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
@@ -9174,20 +9177,20 @@
     </row>
     <row r="101" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
@@ -9211,20 +9214,20 @@
     </row>
     <row r="102" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
@@ -9248,20 +9251,20 @@
     </row>
     <row r="103" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
@@ -9285,13 +9288,13 @@
     </row>
     <row r="104" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D104" s="5"/>
       <c r="E104" s="4"/>
@@ -9318,20 +9321,20 @@
     </row>
     <row r="105" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D105" s="5"/>
       <c r="E105" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G105" s="5"/>
       <c r="H105" s="5"/>
@@ -9355,20 +9358,20 @@
     </row>
     <row r="106" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D106" s="5"/>
       <c r="E106" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
@@ -9392,20 +9395,20 @@
     </row>
     <row r="107" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D107" s="5"/>
       <c r="E107" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G107" s="5"/>
       <c r="H107" s="5"/>
@@ -9429,13 +9432,13 @@
     </row>
     <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D108" s="5"/>
       <c r="E108" s="4"/>
@@ -9462,20 +9465,20 @@
     </row>
     <row r="109" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D109" s="5"/>
       <c r="E109" s="4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G109" s="5"/>
       <c r="H109" s="5"/>
@@ -9499,20 +9502,20 @@
     </row>
     <row r="110" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D110" s="5"/>
       <c r="E110" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G110" s="5"/>
       <c r="H110" s="5"/>
@@ -9536,20 +9539,20 @@
     </row>
     <row r="111" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D111" s="5"/>
       <c r="E111" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G111" s="5"/>
       <c r="H111" s="5"/>
@@ -9573,13 +9576,13 @@
     </row>
     <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D112" s="5"/>
       <c r="E112" s="4"/>
@@ -9606,20 +9609,20 @@
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D113" s="5"/>
       <c r="E113" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G113" s="5"/>
       <c r="H113" s="5"/>
@@ -9643,20 +9646,20 @@
     </row>
     <row r="114" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D114" s="5"/>
       <c r="E114" s="4" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G114" s="5"/>
       <c r="H114" s="5"/>
@@ -9680,20 +9683,20 @@
     </row>
     <row r="115" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D115" s="5"/>
       <c r="E115" s="4" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G115" s="5"/>
       <c r="H115" s="5"/>
@@ -9717,17 +9720,17 @@
     </row>
     <row r="116" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D116" s="5"/>
       <c r="E116" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F116" s="5"/>
       <c r="G116" s="5"/>
@@ -9752,20 +9755,20 @@
     </row>
     <row r="117" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G117" s="11"/>
       <c r="H117" s="11"/>
@@ -9789,20 +9792,20 @@
     </row>
     <row r="118" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D118" s="11"/>
       <c r="E118" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G118" s="11"/>
       <c r="H118" s="11"/>
@@ -9826,20 +9829,20 @@
     </row>
     <row r="119" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D119" s="11"/>
       <c r="E119" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G119" s="11"/>
       <c r="H119" s="11"/>
@@ -9863,13 +9866,13 @@
     </row>
     <row r="120" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D120" s="5"/>
       <c r="E120" s="5"/>
@@ -9896,20 +9899,20 @@
     </row>
     <row r="121" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G121" s="11"/>
       <c r="H121" s="11"/>
@@ -9933,20 +9936,20 @@
     </row>
     <row r="122" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D122" s="11"/>
       <c r="E122" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G122" s="11"/>
       <c r="H122" s="11"/>
@@ -9970,20 +9973,20 @@
     </row>
     <row r="123" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D123" s="11"/>
       <c r="E123" s="4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G123" s="11"/>
       <c r="H123" s="11"/>
@@ -10007,20 +10010,20 @@
     </row>
     <row r="124" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G124" s="4"/>
       <c r="H124" s="4"/>
@@ -10044,20 +10047,20 @@
     </row>
     <row r="125" s="15" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C125" s="13" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D125" s="12"/>
       <c r="E125" s="14" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F125" s="12" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G125" s="12"/>
       <c r="H125" s="12"/>
@@ -10081,17 +10084,17 @@
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C126" s="16" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D126" s="17"/>
       <c r="E126" s="18" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F126" s="16"/>
       <c r="G126" s="16"/>
@@ -10116,20 +10119,20 @@
     </row>
     <row r="127" s="15" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D127" s="12"/>
       <c r="E127" s="14" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F127" s="12" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G127" s="12"/>
       <c r="H127" s="12"/>
@@ -10153,17 +10156,17 @@
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C128" s="16" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D128" s="17"/>
       <c r="E128" s="18" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F128" s="16"/>
       <c r="G128" s="16"/>
@@ -10188,20 +10191,20 @@
     </row>
     <row r="129" s="15" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D129" s="12"/>
       <c r="E129" s="14" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F129" s="12" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G129" s="12"/>
       <c r="H129" s="12"/>
@@ -10225,17 +10228,17 @@
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C130" s="16" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D130" s="17"/>
       <c r="E130" s="18" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F130" s="16"/>
       <c r="G130" s="16"/>
@@ -10292,7 +10295,7 @@
         <v>13</v>
       </c>
       <c r="B132" s="19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C132" s="19" t="s">
         <v>19</v>
@@ -10316,7 +10319,7 @@
         <v>44</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>19</v>
@@ -10327,7 +10330,7 @@
       <c r="G133" s="23"/>
       <c r="H133" s="23"/>
       <c r="I133" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="J133" s="23"/>
       <c r="K133" s="23"/>
@@ -12477,15 +12480,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.6989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>1</v>
@@ -12499,13 +12501,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -12513,13 +12515,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -12551,13 +12553,13 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -12565,13 +12567,13 @@
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -12579,13 +12581,13 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -12601,13 +12603,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -12615,13 +12617,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -12629,13 +12631,13 @@
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -12643,13 +12645,13 @@
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -12665,13 +12667,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -12679,13 +12681,13 @@
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -12693,13 +12695,13 @@
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -12707,13 +12709,13 @@
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -12721,13 +12723,13 @@
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -12743,13 +12745,13 @@
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -12757,13 +12759,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -12771,13 +12773,13 @@
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
@@ -12785,13 +12787,13 @@
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -12799,13 +12801,13 @@
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -12821,13 +12823,13 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -12835,13 +12837,13 @@
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
@@ -12849,13 +12851,13 @@
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -12863,13 +12865,13 @@
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -12877,13 +12879,13 @@
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -12891,13 +12893,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -12905,13 +12907,13 @@
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -12919,13 +12921,13 @@
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -12941,13 +12943,13 @@
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -12955,13 +12957,13 @@
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -12969,13 +12971,13 @@
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -12983,13 +12985,13 @@
     </row>
     <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -12997,13 +12999,13 @@
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -13011,13 +13013,13 @@
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -13025,13 +13027,13 @@
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -13039,13 +13041,13 @@
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -13053,13 +13055,13 @@
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
@@ -13067,13 +13069,13 @@
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -13081,13 +13083,13 @@
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -13103,13 +13105,13 @@
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
@@ -13117,13 +13119,13 @@
     </row>
     <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
@@ -13139,13 +13141,13 @@
     </row>
     <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
@@ -13153,13 +13155,13 @@
     </row>
     <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
@@ -13175,13 +13177,13 @@
     </row>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
@@ -13197,13 +13199,13 @@
     </row>
     <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
@@ -13211,13 +13213,13 @@
     </row>
     <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
@@ -13225,13 +13227,13 @@
     </row>
     <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
@@ -13246,13 +13248,13 @@
     </row>
     <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
@@ -13260,13 +13262,13 @@
     </row>
     <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
@@ -13274,13 +13276,13 @@
     </row>
     <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="B63" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>391</v>
-      </c>
       <c r="C63" s="9" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
@@ -13296,13 +13298,13 @@
     </row>
     <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
@@ -13310,13 +13312,13 @@
     </row>
     <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
@@ -13324,13 +13326,13 @@
     </row>
     <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
@@ -13346,13 +13348,13 @@
     </row>
     <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
@@ -13360,13 +13362,13 @@
     </row>
     <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
@@ -13374,13 +13376,13 @@
     </row>
     <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
@@ -13388,13 +13390,13 @@
     </row>
     <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -13402,13 +13404,13 @@
     </row>
     <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -13416,13 +13418,13 @@
     </row>
     <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
@@ -13430,13 +13432,13 @@
     </row>
     <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
@@ -13472,47 +13474,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.1989795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C2" s="27" t="n">
         <f aca="true">NOW()</f>
-        <v>44067.4618834305</v>
+        <v>44067.5452036865</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="F2" s="9"/>
     </row>

</xml_diff>

<commit_message>
validate date enrolled, art start on linkage form. fix concept for test setting in hts initial and followup forms. fix form logic for contact followup form
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_initial_test.xlsx
+++ b/config/default/forms/app/hts_initial_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -399,7 +399,7 @@
     <t xml:space="preserve">select_one setting</t>
   </si>
   <si>
-    <t xml:space="preserve">test_setting</t>
+    <t xml:space="preserve">_165215_htsSetting_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Setting</t>
@@ -423,7 +423,7 @@
     <t xml:space="preserve">Indicate HTS strategy used?</t>
   </si>
   <si>
-    <t xml:space="preserve">selected(${test_setting},'facility')</t>
+    <t xml:space="preserve">selected(${_165215_htsSetting_99DCT},'_1537_facility_99DCT')</t>
   </si>
   <si>
     <t xml:space="preserve">select_one hts_strategy_community</t>
@@ -432,7 +432,7 @@
     <t xml:space="preserve">community_testing</t>
   </si>
   <si>
-    <t xml:space="preserve">selected(${test_setting},'community')</t>
+    <t xml:space="preserve">selected(${_165215_htsSetting_99DCT},'_163488_community_99DCT')</t>
   </si>
   <si>
     <t xml:space="preserve">_164956_htsStrategyUsed_99DCT</t>
@@ -1424,13 +1424,13 @@
     <t xml:space="preserve">setting</t>
   </si>
   <si>
-    <t xml:space="preserve">community</t>
+    <t xml:space="preserve">_163488_community_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Community</t>
   </si>
   <si>
-    <t xml:space="preserve">facility</t>
+    <t xml:space="preserve">_1537_facility_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Facility</t>
@@ -1890,187 +1890,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+  <dxfs count="79">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -2853,26 +2673,28 @@
   </sheetPr>
   <dimension ref="A1:AL156"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C7" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.7755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="119.780612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.0204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="97.6428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="82.2551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="186.739795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="62.6377551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="59.1275510204082"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="74.7857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.8163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.2959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.5765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="124.102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="101.15306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="193.489795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="64.8877551020408"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="61.1938775510204"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="77.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4721,7 +4543,7 @@
       <c r="X55" s="9"/>
       <c r="Y55" s="9"/>
     </row>
-    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
         <v>124</v>
       </c>
@@ -4791,7 +4613,7 @@
       <c r="X57" s="9"/>
       <c r="Y57" s="9"/>
     </row>
-    <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
         <v>130</v>
       </c>
@@ -4828,7 +4650,7 @@
       <c r="X58" s="9"/>
       <c r="Y58" s="9"/>
     </row>
-    <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
         <v>134</v>
       </c>
@@ -4939,7 +4761,7 @@
       <c r="X61" s="9"/>
       <c r="Y61" s="9"/>
     </row>
-    <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
         <v>142</v>
       </c>
@@ -4976,7 +4798,7 @@
       <c r="X62" s="9"/>
       <c r="Y62" s="9"/>
     </row>
-    <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
         <v>145</v>
       </c>
@@ -10177,508 +9999,536 @@
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E62:E63">
+  <conditionalFormatting sqref="E92">
     <cfRule type="containsText" priority="397" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E62:E63">
+  <conditionalFormatting sqref="E92">
     <cfRule type="expression" priority="398" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A62="begin group", NOT($B62 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62:E63">
+      <formula>AND($A89="begin group", NOT($B89 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E92">
     <cfRule type="expression" priority="399" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A62="end group", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62:E63">
+      <formula>AND($A89="end group", $B89 = "", $C89 = "", $D89 = "", $E89 = "", $F89 = "", $G89 = "", $H89 = "", $I89 = "", $J89 = "", $K89 = "", $L89 = "", $M89 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E92">
     <cfRule type="cellIs" priority="400" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E92">
+    <cfRule type="expression" priority="401" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A89="begin repeat", NOT($B89 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E92">
+    <cfRule type="expression" priority="402" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A89="end repeat", $B89 = "", $C89 = "", $D89 = "", $E89 = "", $F89 = "", $G89 = "", $H89 = "", $I89 = "", $J89 = "", $K89 = "", $L89 = "", $M89 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:Y37">
+    <cfRule type="containsText" priority="403" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:Y37">
+    <cfRule type="cellIs" priority="404" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="cellIs" priority="405" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:Y14">
+    <cfRule type="containsText" priority="406" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:Y14">
+    <cfRule type="expression" priority="407" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A14="begin group", NOT($B14 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:Y14">
+    <cfRule type="expression" priority="408" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A14="end group", $B14 = "", $C14 = "", $D14 = "", $E14 = "", $F14 = "", $G14 = "", $H14 = "", $I14 = "", $J14 = "", $K14 = "", $L14 = "", $M14 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:Y14">
+    <cfRule type="cellIs" priority="409" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14">
+    <cfRule type="expression" priority="410" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($I14 = "", $A14 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" priority="411" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(AND(NOT($A14 = "end group"), NOT($A14 = "end repeat"), NOT($A14 = "")), $C14 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="expression" priority="412" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(AND(NOT($A14 = "end group"), NOT($A14 = "end repeat"), NOT($A14 = "")), $B14 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="cellIs" priority="413" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="expression" priority="414" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(NOT($G14 = ""), $H14 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:Y14">
+    <cfRule type="expression" priority="415" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A14="begin repeat", NOT($B14 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:Y14">
+    <cfRule type="expression" priority="416" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A14="end repeat", $B14 = "", $C14 = "", $D14 = "", $E14 = "", $F14 = "", $G14 = "", $H14 = "", $I14 = "", $J14 = "", $K14 = "", $L14 = "", $M14 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I42">
+    <cfRule type="expression" priority="417" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($I42 = "", $A42 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="containsText" priority="418" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="expression" priority="419" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A42="begin group", NOT($B42 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="expression" priority="420" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A42="end group", $B42 = "", $C42 = "", $D42 = "", $E42 = "", $F42 = "", $G42 = "", $H42 = "", $I42 = "", $J42 = "", $K42 = "", $L42 = "", $M42 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="cellIs" priority="421" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="expression" priority="422" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A42="begin repeat", NOT($B42 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="expression" priority="423" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A42="end repeat", $B42 = "", $C42 = "", $D42 = "", $E42 = "", $F42 = "", $G42 = "", $H42 = "", $I42 = "", $J42 = "", $K42 = "", $L42 = "", $M42 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I65">
+    <cfRule type="expression" priority="424" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($I65 = "", $A65 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" priority="425" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(AND(NOT($A65 = "end group"), NOT($A65 = "end repeat"), NOT($A65 = "")), $C65 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B65">
+    <cfRule type="expression" priority="426" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(AND(NOT($A65 = "end group"), NOT($A65 = "end repeat"), NOT($A65 = "")), $B65 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65">
+    <cfRule type="cellIs" priority="427" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H65">
+    <cfRule type="expression" priority="428" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(NOT($G65 = ""), $H65 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="containsText" priority="429" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="expression" priority="430" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A65="begin group", NOT($B65 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="expression" priority="431" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A65="end group", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="cellIs" priority="432" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="expression" priority="433" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A65="begin repeat", NOT($B65 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="expression" priority="434" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A65="end repeat", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I66">
+    <cfRule type="expression" priority="435" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($I66 = "", $A66 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" priority="436" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $C66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66">
+    <cfRule type="expression" priority="437" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $B66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="cellIs" priority="438" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66">
+    <cfRule type="expression" priority="439" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(NOT($G66 = ""), $H66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="containsText" priority="440" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="441" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A66="begin group", NOT($B66 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="442" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A66="end group", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="cellIs" priority="443" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="444" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A66="begin repeat", NOT($B66 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E66">
+    <cfRule type="expression" priority="445" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($A66="end repeat", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I44">
+    <cfRule type="expression" priority="446" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND($I44 = "", $A44 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" priority="447" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $C44 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44">
+    <cfRule type="expression" priority="448" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $B44 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44">
+    <cfRule type="cellIs" priority="449" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H44">
+    <cfRule type="expression" priority="450" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+      <formula>AND(NOT($G44 = ""), $H44 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="containsText" priority="451" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="expression" priority="452" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+      <formula>AND($A44="begin group", NOT($B44 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="expression" priority="453" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+      <formula>AND($A44="end group", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="cellIs" priority="454" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="expression" priority="455" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+      <formula>AND($A44="begin repeat", NOT($B44 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="expression" priority="456" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+      <formula>AND($A44="end repeat", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I45">
+    <cfRule type="expression" priority="457" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+      <formula>AND($I45 = "", $A45 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45">
+    <cfRule type="expression" priority="458" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+      <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $C45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45">
+    <cfRule type="expression" priority="459" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+      <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $B45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45">
+    <cfRule type="cellIs" priority="460" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45">
+    <cfRule type="expression" priority="461" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
+      <formula>AND(NOT($G45 = ""), $H45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="containsText" priority="462" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="67"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="expression" priority="463" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+      <formula>AND($A45="begin group", NOT($B45 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="expression" priority="464" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+      <formula>AND($A45="end group", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="cellIs" priority="465" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="expression" priority="466" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+      <formula>AND($A45="begin repeat", NOT($B45 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="expression" priority="467" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+      <formula>AND($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I53">
+    <cfRule type="expression" priority="468" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+      <formula>AND($I53 = "", $A53 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="expression" priority="469" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+      <formula>AND(AND(NOT($A53 = "end group"), NOT($A53 = "end repeat"), NOT($A53 = "")), $C53 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A53">
+    <cfRule type="cellIs" priority="470" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53">
+    <cfRule type="expression" priority="471" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+      <formula>AND(NOT($G53 = ""), $H53 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="containsText" priority="472" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="68"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="expression" priority="473" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+      <formula>AND($A53="begin group", NOT($B53 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="expression" priority="474" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+      <formula>AND($A53="end group", $B53 = "", $C53 = "", $D53 = "", $E53 = "", $F53 = "", $G53 = "", $H53 = "", $I53 = "", $J53 = "", $K53 = "", $L53 = "", $M53 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="cellIs" priority="475" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="expression" priority="476" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+      <formula>AND($A53="begin repeat", NOT($B53 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="expression" priority="477" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
+      <formula>AND($A53="end repeat", $B53 = "", $C53 = "", $D53 = "", $E53 = "", $F53 = "", $G53 = "", $H53 = "", $I53 = "", $J53 = "", $K53 = "", $L53 = "", $M53 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:A55">
+    <cfRule type="cellIs" priority="478" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54:E55">
+    <cfRule type="containsText" priority="479" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="71"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54:E55">
+    <cfRule type="cellIs" priority="480" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55:Y55">
+    <cfRule type="containsText" priority="481" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="73"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55:Y55">
+    <cfRule type="cellIs" priority="482" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A55">
+    <cfRule type="cellIs" priority="483" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49">
+    <cfRule type="expression" priority="484" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
+      <formula>COUNTIF($B$2:$B$994,B49)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" priority="485" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1099, "begin group") = COUNTIF($A$1:$A$1099, "end group"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="expression" priority="486" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1090, "begin group") = COUNTIF($A$1:$A$1099, "end group")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I57">
+    <cfRule type="expression" priority="487" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+      <formula>AND($I57 = "", $A57 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57">
+    <cfRule type="expression" priority="488" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+      <formula>AND(AND(NOT($A57 = "end group"), NOT($A57 = "end repeat"), NOT($A57 = "")), $C57 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57">
+    <cfRule type="cellIs" priority="489" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57">
+    <cfRule type="expression" priority="490" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+      <formula>AND(NOT($G57 = ""), $H57 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="containsText" priority="491" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="50"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="expression" priority="492" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+      <formula>AND($A57="begin group", NOT($B57 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="expression" priority="493" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+      <formula>AND($A57="end group", $B57 = "", $C57 = "", $D57 = "", $E57 = "", $F57 = "", $G57 = "", $H57 = "", $I57 = "", $J57 = "", $K57 = "", $L57 = "", $M57 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="cellIs" priority="494" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="expression" priority="495" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+      <formula>AND($A57="begin repeat", NOT($B57 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="expression" priority="496" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+      <formula>AND($A57="end repeat", $B57 = "", $C57 = "", $D57 = "", $E57 = "", $F57 = "", $G57 = "", $H57 = "", $I57 = "", $J57 = "", $K57 = "", $L57 = "", $M57 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E59">
+    <cfRule type="containsText" priority="497" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E59">
+    <cfRule type="expression" priority="498" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A58="begin group", NOT($B58 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E59">
+    <cfRule type="expression" priority="499" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A58="end group", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E59">
+    <cfRule type="cellIs" priority="500" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E59">
+    <cfRule type="expression" priority="501" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A58="begin repeat", NOT($B58 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58:E59">
+    <cfRule type="expression" priority="502" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A58="end repeat", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E62:E63">
-    <cfRule type="expression" priority="401" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="containsText" priority="503" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62:E63">
+    <cfRule type="expression" priority="504" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A62="begin group", NOT($B62 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62:E63">
+    <cfRule type="expression" priority="505" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND($A62="end group", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62:E63">
+    <cfRule type="cellIs" priority="506" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62:E63">
+    <cfRule type="expression" priority="507" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>AND($A62="begin repeat", NOT($B62 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E63">
-    <cfRule type="expression" priority="402" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="508" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>AND($A62="end repeat", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="containsText" priority="403" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="expression" priority="404" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A89="begin group", NOT($B89 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="expression" priority="405" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A89="end group", $B89 = "", $C89 = "", $D89 = "", $E89 = "", $F89 = "", $G89 = "", $H89 = "", $I89 = "", $J89 = "", $K89 = "", $L89 = "", $M89 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" priority="406" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="expression" priority="407" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A89="begin repeat", NOT($B89 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="expression" priority="408" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A89="end repeat", $B89 = "", $C89 = "", $D89 = "", $E89 = "", $F89 = "", $G89 = "", $H89 = "", $I89 = "", $J89 = "", $K89 = "", $L89 = "", $M89 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:Y37">
-    <cfRule type="containsText" priority="409" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:Y37">
-    <cfRule type="cellIs" priority="410" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
-    <cfRule type="cellIs" priority="411" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="containsText" priority="412" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="expression" priority="413" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A14="begin group", NOT($B14 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="expression" priority="414" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A14="end group", $B14 = "", $C14 = "", $D14 = "", $E14 = "", $F14 = "", $G14 = "", $H14 = "", $I14 = "", $J14 = "", $K14 = "", $L14 = "", $M14 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="cellIs" priority="415" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14">
-    <cfRule type="expression" priority="416" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($I14 = "", $A14 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" priority="417" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND(AND(NOT($A14 = "end group"), NOT($A14 = "end repeat"), NOT($A14 = "")), $C14 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="expression" priority="418" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND(AND(NOT($A14 = "end group"), NOT($A14 = "end repeat"), NOT($A14 = "")), $B14 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" priority="419" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
-    <cfRule type="expression" priority="420" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND(NOT($G14 = ""), $H14 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="expression" priority="421" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A14="begin repeat", NOT($B14 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="expression" priority="422" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A14="end repeat", $B14 = "", $C14 = "", $D14 = "", $E14 = "", $F14 = "", $G14 = "", $H14 = "", $I14 = "", $J14 = "", $K14 = "", $L14 = "", $M14 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I42">
-    <cfRule type="expression" priority="423" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($I42 = "", $A42 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" priority="424" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="expression" priority="425" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A42="begin group", NOT($B42 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="expression" priority="426" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A42="end group", $B42 = "", $C42 = "", $D42 = "", $E42 = "", $F42 = "", $G42 = "", $H42 = "", $I42 = "", $J42 = "", $K42 = "", $L42 = "", $M42 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" priority="427" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="expression" priority="428" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A42="begin repeat", NOT($B42 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="expression" priority="429" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($A42="end repeat", $B42 = "", $C42 = "", $D42 = "", $E42 = "", $F42 = "", $G42 = "", $H42 = "", $I42 = "", $J42 = "", $K42 = "", $L42 = "", $M42 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I65">
-    <cfRule type="expression" priority="430" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND($I65 = "", $A65 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" priority="431" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND(AND(NOT($A65 = "end group"), NOT($A65 = "end repeat"), NOT($A65 = "")), $C65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B65">
-    <cfRule type="expression" priority="432" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND(AND(NOT($A65 = "end group"), NOT($A65 = "end repeat"), NOT($A65 = "")), $B65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="cellIs" priority="433" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H65">
-    <cfRule type="expression" priority="434" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
-      <formula>AND(NOT($G65 = ""), $H65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="containsText" priority="435" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="expression" priority="436" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND($A65="begin group", NOT($B65 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="expression" priority="437" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND($A65="end group", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" priority="438" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="expression" priority="439" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND($A65="begin repeat", NOT($B65 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="expression" priority="440" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND($A65="end repeat", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I66">
-    <cfRule type="expression" priority="441" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND($I66 = "", $A66 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
-    <cfRule type="expression" priority="442" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $C66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B66">
-    <cfRule type="expression" priority="443" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $B66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="cellIs" priority="444" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H66">
-    <cfRule type="expression" priority="445" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
-      <formula>AND(NOT($G66 = ""), $H66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="containsText" priority="446" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="66"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="447" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
-      <formula>AND($A66="begin group", NOT($B66 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="448" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
-      <formula>AND($A66="end group", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" priority="449" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="450" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
-      <formula>AND($A66="begin repeat", NOT($B66 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="451" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
-      <formula>AND($A66="end repeat", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I44">
-    <cfRule type="expression" priority="452" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
-      <formula>AND($I44 = "", $A44 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="expression" priority="453" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
-      <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $C44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
-    <cfRule type="expression" priority="454" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
-      <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $B44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44">
-    <cfRule type="cellIs" priority="455" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H44">
-    <cfRule type="expression" priority="456" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
-      <formula>AND(NOT($G44 = ""), $H44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" priority="457" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="68"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="expression" priority="458" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
-      <formula>AND($A44="begin group", NOT($B44 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="expression" priority="459" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
-      <formula>AND($A44="end group", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" priority="460" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="expression" priority="461" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
-      <formula>AND($A44="begin repeat", NOT($B44 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="expression" priority="462" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
-      <formula>AND($A44="end repeat", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I45">
-    <cfRule type="expression" priority="463" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
-      <formula>AND($I45 = "", $A45 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="expression" priority="464" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
-      <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $C45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45">
-    <cfRule type="expression" priority="465" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
-      <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $B45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45">
-    <cfRule type="cellIs" priority="466" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H45">
-    <cfRule type="expression" priority="467" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
-      <formula>AND(NOT($G45 = ""), $H45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" priority="468" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="79"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="expression" priority="469" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
-      <formula>AND($A45="begin group", NOT($B45 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="expression" priority="470" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
-      <formula>AND($A45="end group", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="cellIs" priority="471" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="expression" priority="472" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
-      <formula>AND($A45="begin repeat", NOT($B45 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="expression" priority="473" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
-      <formula>AND($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I53">
-    <cfRule type="expression" priority="474" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
-      <formula>AND($I53 = "", $A53 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="expression" priority="475" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
-      <formula>AND(AND(NOT($A53 = "end group"), NOT($A53 = "end repeat"), NOT($A53 = "")), $C53 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" priority="476" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H53">
-    <cfRule type="expression" priority="477" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
-      <formula>AND(NOT($G53 = ""), $H53 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="containsText" priority="478" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="87"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="expression" priority="479" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
-      <formula>AND($A53="begin group", NOT($B53 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="expression" priority="480" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
-      <formula>AND($A53="end group", $B53 = "", $C53 = "", $D53 = "", $E53 = "", $F53 = "", $G53 = "", $H53 = "", $I53 = "", $J53 = "", $K53 = "", $L53 = "", $M53 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" priority="481" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="expression" priority="482" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
-      <formula>AND($A53="begin repeat", NOT($B53 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="expression" priority="483" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
-      <formula>AND($A53="end repeat", $B53 = "", $C53 = "", $D53 = "", $E53 = "", $F53 = "", $G53 = "", $H53 = "", $I53 = "", $J53 = "", $K53 = "", $L53 = "", $M53 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:A55">
-    <cfRule type="cellIs" priority="484" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E54:E55">
-    <cfRule type="containsText" priority="485" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="91"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E54:E55">
-    <cfRule type="cellIs" priority="486" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="containsText" priority="487" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="93"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="cellIs" priority="488" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A55">
-    <cfRule type="cellIs" priority="489" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B49">
-    <cfRule type="expression" priority="490" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
-      <formula>COUNTIF($B$2:$B$994,B49)&gt;1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="491" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$1099, "begin group") = COUNTIF($A$1:$A$1099, "end group"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="492" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1090, "begin group") = COUNTIF($A$1:$A$1099, "end group")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I57">
-    <cfRule type="expression" priority="493" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND($I57 = "", $A57 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="expression" priority="494" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND(AND(NOT($A57 = "end group"), NOT($A57 = "end repeat"), NOT($A57 = "")), $C57 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
-    <cfRule type="cellIs" priority="495" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>"hidden"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H57">
-    <cfRule type="expression" priority="496" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND(NOT($G57 = ""), $H57 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="containsText" priority="497" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="50"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="498" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND($A57="begin group", NOT($B57 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="499" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND($A57="end group", $B57 = "", $C57 = "", $D57 = "", $E57 = "", $F57 = "", $G57 = "", $H57 = "", $I57 = "", $J57 = "", $K57 = "", $L57 = "", $M57 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" priority="500" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>"note"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="501" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND($A57="begin repeat", NOT($B57 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="502" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND($A57="end repeat", $B57 = "", $C57 = "", $D57 = "", $E57 = "", $F57 = "", $G57 = "", $H57 = "", $I57 = "", $J57 = "", $K57 = "", $L57 = "", $M57 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -10708,16 +10558,17 @@
   <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="63.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="77.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="98.8163265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.6071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="102.413265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11901,22 +11752,22 @@
       <c r="E94" s="13"/>
       <c r="F94" s="13"/>
     </row>
-    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>465</v>
       </c>
-      <c r="B96" s="0" t="s">
+      <c r="B96" s="30" t="s">
         <v>466</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>465</v>
       </c>
-      <c r="B97" s="0" t="s">
+      <c r="B97" s="30" t="s">
         <v>468</v>
       </c>
       <c r="C97" s="0" t="s">
@@ -12279,7 +12130,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.0561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12311,7 +12164,7 @@
       </c>
       <c r="C2" s="32" t="n">
         <f aca="true">NOW()</f>
-        <v>44279.9137037207</v>
+        <v>44281.3987149428</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>505</v>

</xml_diff>

<commit_message>
make phone number in contact listing form optional. correct concept for pmtct-anc in initial and followup forms. add variable for consent in retest form and display response on clients profile
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_initial_test.xlsx
+++ b/config/default/forms/app/hts_initial_test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="513">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -1439,13 +1439,31 @@
     <t xml:space="preserve">entry_point_facility</t>
   </si>
   <si>
-    <t xml:space="preserve">_162223_emergency_99DCT</t>
+    <t xml:space="preserve">_160538_pmtctAnc_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMTCT – ANC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_160456_pmtctMat_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMTCT – MAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_1623_pmtctPnc_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMTCT – PNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_162223_vmmc_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">VMMC</t>
   </si>
   <si>
-    <t xml:space="preserve">_160522_vmmc_99DCT</t>
+    <t xml:space="preserve">_160522_emergency_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Emergency</t>
@@ -1890,565 +1908,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="79">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -2673,28 +2133,26 @@
   </sheetPr>
   <dimension ref="A1:AL156"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C7" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="topRight" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.8163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.2959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.5765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.780612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="124.102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="101.15306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="85.2244897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="193.489795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="64.8877551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="61.1938775510204"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="77.484693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.7755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.2448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="138.051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="112.581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="94.765306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="215.357142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="71.9948979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="67.9438775510204"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="86.2142857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8382,2152 +7840,2152 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H133">
-    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="expression" priority="59" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(NOT($G133 = ""), $H133 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135:Y135">
-    <cfRule type="containsText" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="2"/>
+    <cfRule type="containsText" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135:Y135">
-    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A135="begin group", NOT($B135 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135:Y135">
-    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A135="end group", $B135 = "", $C135 = "", $D135 = "", $E135 = "", $F135 = "", $G135 = "", $H135 = "", $I135 = "", $J135 = "", $K135 = "", $L135 = "", $M135 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135:Y135">
-    <cfRule type="cellIs" priority="63" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" priority="63" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I135">
-    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="64" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($I135 = "", $A135 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C135">
-    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A135 = "end group"), NOT($A135 = "end repeat"), NOT($A135 = "")), $C135 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B135">
-    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A135 = "end group"), NOT($A135 = "end repeat"), NOT($A135 = "")), $B135 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135">
-    <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H135">
-    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(NOT($G135 = ""), $H135 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135:Y135">
-    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A135="begin repeat", NOT($B135 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A135:Y135">
-    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="70" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A135="end repeat", $B135 = "", $C135 = "", $D135 = "", $E135 = "", $F135 = "", $G135 = "", $H135 = "", $I135 = "", $J135 = "", $K135 = "", $L135 = "", $M135 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:Y136">
-    <cfRule type="containsText" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="4"/>
+    <cfRule type="containsText" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:Y136">
-    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A136="begin group", NOT($B136 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:Y136">
-    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="73" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A136="end group", $B136 = "", $C136 = "", $D136 = "", $E136 = "", $F136 = "", $G136 = "", $H136 = "", $I136 = "", $J136 = "", $K136 = "", $L136 = "", $M136 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:Y136">
-    <cfRule type="cellIs" priority="74" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="74" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I136">
-    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="75" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($I136 = "", $A136 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C136">
-    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="76" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A136 = "end group"), NOT($A136 = "end repeat"), NOT($A136 = "")), $C136 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B136">
-    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="77" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A136 = "end group"), NOT($A136 = "end repeat"), NOT($A136 = "")), $B136 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136">
-    <cfRule type="cellIs" priority="78" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="78" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136">
-    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="expression" priority="79" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(NOT($G136 = ""), $H136 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:Y136">
-    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="80" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A136="begin repeat", NOT($B136 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A136:Y136">
-    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="81" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A136="end repeat", $B136 = "", $C136 = "", $D136 = "", $E136 = "", $F136 = "", $G136 = "", $H136 = "", $I136 = "", $J136 = "", $K136 = "", $L136 = "", $M136 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137:Y137">
-    <cfRule type="containsText" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="6"/>
+    <cfRule type="containsText" priority="82" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137:Y137">
-    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="83" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A137="begin group", NOT($B137 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137:Y137">
-    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="84" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A137="end group", $B137 = "", $C137 = "", $D137 = "", $E137 = "", $F137 = "", $G137 = "", $H137 = "", $I137 = "", $J137 = "", $K137 = "", $L137 = "", $M137 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137:Y137">
-    <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I137">
-    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="86" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($I137 = "", $A137 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C137">
-    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="expression" priority="87" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A137 = "end group"), NOT($A137 = "end repeat"), NOT($A137 = "")), $C137 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B137">
-    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="expression" priority="88" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A137 = "end group"), NOT($A137 = "end repeat"), NOT($A137 = "")), $B137 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137">
-    <cfRule type="cellIs" priority="89" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="cellIs" priority="89" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H137">
-    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="90" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(NOT($G137 = ""), $H137 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137:Y137">
-    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="91" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A137="begin repeat", NOT($B137 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A137:Y137">
-    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="92" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A137="end repeat", $B137 = "", $C137 = "", $D137 = "", $E137 = "", $F137 = "", $G137 = "", $H137 = "", $I137 = "", $J137 = "", $K137 = "", $L137 = "", $M137 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:Y142">
-    <cfRule type="containsText" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="9"/>
+    <cfRule type="containsText" priority="93" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:Y142">
-    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="94" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A142="begin group", NOT($B142 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:Y142">
-    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="95" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A142="end group", $B142 = "", $C142 = "", $D142 = "", $E142 = "", $F142 = "", $G142 = "", $H142 = "", $I142 = "", $J142 = "", $K142 = "", $L142 = "", $M142 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:Y142">
-    <cfRule type="cellIs" priority="96" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="96" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I142">
-    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="expression" priority="97" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($I142 = "", $A142 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C142">
-    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="98" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A142 = "end group"), NOT($A142 = "end repeat"), NOT($A142 = "")), $C142 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B142">
-    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="99" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A142 = "end group"), NOT($A142 = "end repeat"), NOT($A142 = "")), $B142 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142">
-    <cfRule type="cellIs" priority="100" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="cellIs" priority="100" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H142">
-    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="101" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(NOT($G142 = ""), $H142 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:Y142">
-    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="102" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A142="begin repeat", NOT($B142 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:Y142">
-    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="103" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A142="end repeat", $B142 = "", $C142 = "", $D142 = "", $E142 = "", $F142 = "", $G142 = "", $H142 = "", $I142 = "", $J142 = "", $K142 = "", $L142 = "", $M142 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="containsText" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="12"/>
+    <cfRule type="containsText" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A153="begin group", NOT($B153 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A153="end group", $B153 = "", $C153 = "", $D153 = "", $E153 = "", $F153 = "", $G153 = "", $H153 = "", $I153 = "", $J153 = "", $K153 = "", $L153 = "", $M153 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="cellIs" priority="107" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="cellIs" priority="107" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="cellIs" priority="108" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="cellIs" priority="108" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A153="begin repeat", NOT($B153 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A153">
-    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A153="end repeat", $B153 = "", $C153 = "", $D153 = "", $E153 = "", $F153 = "", $G153 = "", $H153 = "", $I153 = "", $J153 = "", $K153 = "", $L153 = "", $M153 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I139:I141">
-    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($I139 = "", $A139 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C140:C141">
-    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A140 = "end group"), NOT($A140 = "end repeat"), NOT($A140 = "")), $C140 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B140:B141">
-    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A140 = "end group"), NOT($A140 = "end repeat"), NOT($A140 = "")), $B140 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A139:A141">
-    <cfRule type="cellIs" priority="114" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="cellIs" priority="114" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H139:H141">
-    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(NOT($G139 = ""), $H139 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138:Y138">
-    <cfRule type="containsText" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="12"/>
+    <cfRule type="containsText" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138:Y138">
-    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A138="begin group", NOT($B138 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138:Y138">
-    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="118" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A138="end group", $B138 = "", $C138 = "", $D138 = "", $E138 = "", $F138 = "", $G138 = "", $H138 = "", $I138 = "", $J138 = "", $K138 = "", $L138 = "", $M138 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138:Y138">
-    <cfRule type="cellIs" priority="119" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="cellIs" priority="119" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I138">
-    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="120" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($I138 = "", $A138 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C138">
-    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="121" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A138 = "end group"), NOT($A138 = "end repeat"), NOT($A138 = "")), $C138 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B138">
-    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="expression" priority="122" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A138 = "end group"), NOT($A138 = "end repeat"), NOT($A138 = "")), $B138 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138">
-    <cfRule type="cellIs" priority="123" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="cellIs" priority="123" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H138">
-    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="expression" priority="124" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(NOT($G138 = ""), $H138 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138:Y138">
-    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="expression" priority="125" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A138="begin repeat", NOT($B138 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A138:Y138">
-    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
+    <cfRule type="expression" priority="126" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A138="end repeat", $B138 = "", $C138 = "", $D138 = "", $E138 = "", $F138 = "", $G138 = "", $H138 = "", $I138 = "", $J138 = "", $K138 = "", $L138 = "", $M138 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="containsText" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="18"/>
+    <cfRule type="containsText" priority="127" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="expression" priority="128" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A130="begin group", NOT($B130 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
+    <cfRule type="expression" priority="129" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A130="end group", $B130 = "", $C130 = "", $D130 = "", $E130 = "", $F130 = "", $G130 = "", $H130 = "", $I130 = "", $J130 = "", $K130 = "", $L130 = "", $M130 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="cellIs" priority="130" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+    <cfRule type="cellIs" priority="130" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+    <cfRule type="expression" priority="131" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A130="begin repeat", NOT($B130 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="23">
+    <cfRule type="expression" priority="132" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A130="end repeat", $B130 = "", $C130 = "", $D130 = "", $E130 = "", $F130 = "", $G130 = "", $H130 = "", $I130 = "", $J130 = "", $K130 = "", $L130 = "", $M130 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="containsText" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="24"/>
+    <cfRule type="containsText" priority="133" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+    <cfRule type="expression" priority="134" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A130="begin group", NOT($B130 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
+    <cfRule type="expression" priority="135" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A130="end group", $B130 = "", $C130 = "", $D130 = "", $E130 = "", $F130 = "", $G130 = "", $H130 = "", $I130 = "", $J130 = "", $K130 = "", $L130 = "", $M130 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="cellIs" priority="136" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+    <cfRule type="cellIs" priority="136" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+    <cfRule type="expression" priority="137" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A130="begin repeat", NOT($B130 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+    <cfRule type="expression" priority="138" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A130="end repeat", $B130 = "", $C130 = "", $D130 = "", $E130 = "", $F130 = "", $G130 = "", $H130 = "", $I130 = "", $J130 = "", $K130 = "", $L130 = "", $M130 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I130">
-    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+    <cfRule type="expression" priority="139" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($I130 = "", $A130 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C130">
-    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+    <cfRule type="expression" priority="140" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A130 = "end group"), NOT($A130 = "end repeat"), NOT($A130 = "")), $C130 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B130">
-    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+    <cfRule type="expression" priority="141" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND(AND(NOT($A130 = "end group"), NOT($A130 = "end repeat"), NOT($A130 = "")), $B130 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A130">
-    <cfRule type="cellIs" priority="142" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+    <cfRule type="cellIs" priority="142" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H130">
-    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+    <cfRule type="expression" priority="143" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G130 = ""), $H130 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="containsText" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="35"/>
+    <cfRule type="containsText" priority="144" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+    <cfRule type="expression" priority="145" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A134="begin group", NOT($B134 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+    <cfRule type="expression" priority="146" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A134="end group", $B134 = "", $C134 = "", $D134 = "", $E134 = "", $F134 = "", $G134 = "", $H134 = "", $I134 = "", $J134 = "", $K134 = "", $L134 = "", $M134 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="cellIs" priority="147" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+    <cfRule type="cellIs" priority="147" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+    <cfRule type="expression" priority="148" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A134="begin repeat", NOT($B134 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+    <cfRule type="expression" priority="149" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A134="end repeat", $B134 = "", $C134 = "", $D134 = "", $E134 = "", $F134 = "", $G134 = "", $H134 = "", $I134 = "", $J134 = "", $K134 = "", $L134 = "", $M134 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="containsText" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="41"/>
+    <cfRule type="containsText" priority="150" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+    <cfRule type="expression" priority="151" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A134="begin group", NOT($B134 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+    <cfRule type="expression" priority="152" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A134="end group", $B134 = "", $C134 = "", $D134 = "", $E134 = "", $F134 = "", $G134 = "", $H134 = "", $I134 = "", $J134 = "", $K134 = "", $L134 = "", $M134 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="cellIs" priority="153" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+    <cfRule type="cellIs" priority="153" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
+    <cfRule type="expression" priority="154" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A134="begin repeat", NOT($B134 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E134">
-    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
+    <cfRule type="expression" priority="155" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A134="end repeat", $B134 = "", $C134 = "", $D134 = "", $E134 = "", $F134 = "", $G134 = "", $H134 = "", $I134 = "", $J134 = "", $K134 = "", $L134 = "", $M134 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I134">
-    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="expression" priority="156" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I134 = "", $A134 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C134">
-    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="expression" priority="157" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A134 = "end group"), NOT($A134 = "end repeat"), NOT($A134 = "")), $C134 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B134">
-    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="expression" priority="158" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A134 = "end group"), NOT($A134 = "end repeat"), NOT($A134 = "")), $B134 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A134">
-    <cfRule type="cellIs" priority="159" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="cellIs" priority="159" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H134">
-    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="expression" priority="160" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G134 = ""), $H134 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="containsText" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="45"/>
+    <cfRule type="containsText" priority="161" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="expression" priority="162" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A41="begin group", NOT($B41 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
+    <cfRule type="expression" priority="163" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A41="end group", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="cellIs" priority="164" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
+    <cfRule type="cellIs" priority="164" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
+    <cfRule type="expression" priority="165" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A41="begin repeat", NOT($B41 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
+    <cfRule type="expression" priority="166" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A41="end repeat", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46">
-    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="167" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I46 = "", $A46 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:C47">
-    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="168" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A46 = "end group"), NOT($A46 = "end repeat"), NOT($A46 = "")), $C46 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:A47">
-    <cfRule type="cellIs" priority="169" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="cellIs" priority="169" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46:H47">
-    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="170" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G46 = ""), $H46 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:E47">
-    <cfRule type="containsText" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="49"/>
+    <cfRule type="containsText" priority="171" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:E47">
-    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="172" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A46="begin group", NOT($B46 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:E47">
-    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="173" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A46="end group", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:E47">
-    <cfRule type="cellIs" priority="174" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="cellIs" priority="174" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:E47">
-    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="175" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A46="begin repeat", NOT($B46 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:E47">
-    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
+    <cfRule type="expression" priority="176" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A46="end repeat", $B46 = "", $C46 = "", $D46 = "", $E46 = "", $F46 = "", $G46 = "", $H46 = "", $I46 = "", $J46 = "", $K46 = "", $L46 = "", $M46 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="containsText" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="50"/>
+    <cfRule type="containsText" priority="177" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="178" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A51="begin group", NOT($B51 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A51="end group", $B51 = "", $C51 = "", $D51 = "", $E51 = "", $F51 = "", $G51 = "", $H51 = "", $I51 = "", $J51 = "", $K51 = "", $L51 = "", $M51 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" priority="180" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="cellIs" priority="180" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A51="begin repeat", NOT($B51 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A51="end repeat", $B51 = "", $C51 = "", $D51 = "", $E51 = "", $F51 = "", $G51 = "", $H51 = "", $I51 = "", $J51 = "", $K51 = "", $L51 = "", $M51 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A50 = "end group"), NOT($A50 = "end repeat"), NOT($A50 = "")), $C50 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50">
-    <cfRule type="cellIs" priority="184" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="cellIs" priority="184" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G50 = ""), $H50 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="containsText" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="50"/>
+    <cfRule type="containsText" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A50="begin group", NOT($B50 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A50="end group", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $I50 = "", $M50 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="cellIs" priority="189" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="cellIs" priority="189" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A50="begin repeat", NOT($B50 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A50="end repeat", $B50 = "", $C50 = "", $D50 = "", $E50 = "", $F50 = "", $G50 = "", $H50 = "", $I50 = "", $J50 = "", $K50 = "", $I50 = "", $M50 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="containsText" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="50"/>
+    <cfRule type="containsText" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="193" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A48="begin group", NOT($B48 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="194" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A48="end group", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $I48 = "", $M48 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="cellIs" priority="195" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="cellIs" priority="195" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="196" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A48="begin repeat", NOT($B48 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48">
-    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="197" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A48="end repeat", $B48 = "", $C48 = "", $D48 = "", $E48 = "", $F48 = "", $G48 = "", $H48 = "", $I48 = "", $J48 = "", $K48 = "", $I48 = "", $M48 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I60">
-    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="198" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I60 = "", $A60 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="199" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A60 = "end group"), NOT($A60 = "end repeat"), NOT($A60 = "")), $C60 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="cellIs" priority="200" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="cellIs" priority="200" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60">
-    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="201" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G60 = ""), $H60 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="containsText" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="50"/>
+    <cfRule type="containsText" priority="202" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
+    <cfRule type="expression" priority="203" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A60="begin group", NOT($B60 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
+    <cfRule type="expression" priority="204" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A60="end group", $B60 = "", $C60 = "", $D60 = "", $E60 = "", $F60 = "", $G60 = "", $H60 = "", $I60 = "", $J60 = "", $K60 = "", $L60 = "", $M60 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" priority="205" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
+    <cfRule type="cellIs" priority="205" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="206" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A60="begin repeat", NOT($B60 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="207" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A60="end repeat", $B60 = "", $C60 = "", $D60 = "", $E60 = "", $F60 = "", $G60 = "", $H60 = "", $I60 = "", $J60 = "", $K60 = "", $L60 = "", $M60 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67">
-    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="208" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I67 = "", $A67 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="expression" priority="209" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="209" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A67 = "end group"), NOT($A67 = "end repeat"), NOT($A67 = "")), $C67 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="cellIs" priority="210" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="cellIs" priority="210" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H67">
-    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="211" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G67 = ""), $H67 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="containsText" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="54"/>
+    <cfRule type="containsText" priority="212" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="213" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A67="begin group", NOT($B67 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="214" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A67="end group", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" priority="215" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="cellIs" priority="215" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="216" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A67="begin repeat", NOT($B67 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="217" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A67="end repeat", $B67 = "", $C67 = "", $D67 = "", $E67 = "", $F67 = "", $G67 = "", $H67 = "", $I67 = "", $J67 = "", $K67 = "", $L67 = "", $M67 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I68:I69">
-    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="218" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I68 = "", $A68 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C69">
-    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="219" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $C68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68:B69">
-    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="220" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A68 = "end group"), NOT($A68 = "end repeat"), NOT($A68 = "")), $B68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68:A69">
-    <cfRule type="cellIs" priority="221" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="cellIs" priority="221" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68:H69">
-    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
+    <cfRule type="expression" priority="222" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G68 = ""), $H68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68:E69">
-    <cfRule type="containsText" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="55"/>
+    <cfRule type="containsText" priority="223" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68:E69">
-    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="224" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A68="begin group", NOT($B68 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68:E69">
-    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="225" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A68="end group", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68:E69">
-    <cfRule type="cellIs" priority="226" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="cellIs" priority="226" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68:E69">
-    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="227" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A68="begin repeat", NOT($B68 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68:E69">
-    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="228" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A68="end repeat", $B68 = "", $C68 = "", $D68 = "", $E68 = "", $F68 = "", $G68 = "", $H68 = "", $I68 = "", $J68 = "", $K68 = "", $L68 = "", $M68 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64">
-    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="229" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I64 = "", $A64 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="230" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A64 = "end group"), NOT($A64 = "end repeat"), NOT($A64 = "")), $C64 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:A64">
-    <cfRule type="cellIs" priority="231" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="cellIs" priority="231" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H64">
-    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
+    <cfRule type="expression" priority="232" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G64 = ""), $H64 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="containsText" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="233" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="234" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A64="begin group", NOT($B64 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="235" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A64="end group", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $I64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="cellIs" priority="236" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="236" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="237" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A64="begin repeat", NOT($B64 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="238" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A64="end repeat", $B64 = "", $C64 = "", $D64 = "", $E64 = "", $F64 = "", $G64 = "", $H64 = "", $I64 = "", $J64 = "", $K64 = "", $L64 = "", $M64 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A71">
-    <cfRule type="cellIs" priority="239" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="239" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:Y74">
-    <cfRule type="containsText" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="240" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:Y74">
-    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="241" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A72="begin group", NOT($B72 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:Y74">
-    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="242" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A72="end group", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:Y74">
-    <cfRule type="cellIs" priority="243" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="243" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I72:I74">
-    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="244" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I72 = "", $A72 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72:C74">
-    <cfRule type="expression" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="245" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A72 = "end group"), NOT($A72 = "end repeat"), NOT($A72 = "")), $C72 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72:B74">
-    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="246" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A72 = "end group"), NOT($A72 = "end repeat"), NOT($A72 = "")), $B72 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:A74">
-    <cfRule type="cellIs" priority="247" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="247" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72:H74">
-    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="248" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G72 = ""), $H72 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:Y74">
-    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="249" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A72="begin repeat", NOT($B72 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:Y74">
-    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="250" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A72="end repeat", $B72 = "", $C72 = "", $D72 = "", $E72 = "", $F72 = "", $G72 = "", $H72 = "", $I72 = "", $J72 = "", $K72 = "", $L72 = "", $M72 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="containsText" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="251" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="252" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A77="begin group", NOT($B77 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="253" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A77="end group", $B77 = "", $C77 = "", $D77 = "", $E77 = "", $F77 = "", $G77 = "", $H77 = "", $I77 = "", $J77 = "", $K77 = "", $L77 = "", $M77 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="cellIs" priority="254" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="254" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="cellIs" priority="255" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="255" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="256" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A77="begin repeat", NOT($B77 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A77">
-    <cfRule type="expression" priority="257" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="257" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A77="end repeat", $B77 = "", $C77 = "", $D77 = "", $E77 = "", $F77 = "", $G77 = "", $H77 = "", $I77 = "", $J77 = "", $K77 = "", $L77 = "", $M77 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="containsText" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="258" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="259" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A77="begin group", NOT($B77 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="260" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A77="end group", $B77 = "", $C77 = "", $D77 = "", $E77 = "", $F77 = "", $G77 = "", $H77 = "", $I77 = "", $J77 = "", $K77 = "", $L77 = "", $M77 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="cellIs" priority="261" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="261" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="262" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A77="begin repeat", NOT($B77 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E77">
-    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="263" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A77="end repeat", $B77 = "", $C77 = "", $D77 = "", $E77 = "", $F77 = "", $G77 = "", $H77 = "", $I77 = "", $J77 = "", $K77 = "", $L77 = "", $M77 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A78">
-    <cfRule type="cellIs" priority="264" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="264" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I79:I81">
-    <cfRule type="expression" priority="265" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="265" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I79 = "", $A79 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79:C81">
-    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="266" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A79 = "end group"), NOT($A79 = "end repeat"), NOT($A79 = "")), $C79 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B81">
-    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="267" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A80 = "end group"), NOT($A80 = "end repeat"), NOT($A80 = "")), $B80 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A79:A81">
-    <cfRule type="cellIs" priority="268" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="268" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79:H81">
-    <cfRule type="expression" priority="269" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="269" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G79 = ""), $H79 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I87">
-    <cfRule type="expression" priority="270" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="270" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I87 = "", $A87 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="expression" priority="271" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="271" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A87 = "end group"), NOT($A87 = "end repeat"), NOT($A87 = "")), $C87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="expression" priority="272" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="272" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A87 = "end group"), NOT($A87 = "end repeat"), NOT($A87 = "")), $B87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A87">
-    <cfRule type="cellIs" priority="273" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="273" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87">
-    <cfRule type="expression" priority="274" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="274" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G87 = ""), $H87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="containsText" priority="275" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="275" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" priority="276" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="276" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A87="begin group", NOT($B87 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" priority="277" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="277" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A87="end group", $B87 = "", $C87 = "", $D87 = "", $E87 = "", $F87 = "", $G87 = "", $H87 = "", $I87 = "", $J87 = "", $K87 = "", $L87 = "", $M87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="cellIs" priority="278" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="278" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" priority="279" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="279" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A87="begin repeat", NOT($B87 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87">
-    <cfRule type="expression" priority="280" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="280" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A87="end repeat", $B87 = "", $C87 = "", $D87 = "", $E87 = "", $F87 = "", $G87 = "", $H87 = "", $I87 = "", $J87 = "", $K87 = "", $L87 = "", $M87 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I88:I94">
-    <cfRule type="expression" priority="281" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="281" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I88 = "", $A88 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C94">
-    <cfRule type="expression" priority="282" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="282" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A88 = "end group"), NOT($A88 = "end repeat"), NOT($A88 = "")), $C88 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A88:A94">
-    <cfRule type="cellIs" priority="283" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="283" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88:H94">
-    <cfRule type="expression" priority="284" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="284" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G88 = ""), $H88 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="containsText" priority="285" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="285" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="expression" priority="286" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="286" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A82="begin group", NOT($B82 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="expression" priority="287" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="287" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A82="end group", $B82 = "", $C82 = "", $D82 = "", $E82 = "", $F82 = "", $G82 = "", $H82 = "", $I82 = "", $J82 = "", $K82 = "", $L82 = "", $M82 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="cellIs" priority="288" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="288" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="cellIs" priority="289" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="289" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="expression" priority="290" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="290" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A82="begin repeat", NOT($B82 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="expression" priority="291" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="291" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A82="end repeat", $B82 = "", $C82 = "", $D82 = "", $E82 = "", $F82 = "", $G82 = "", $H82 = "", $I82 = "", $J82 = "", $K82 = "", $L82 = "", $M82 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43">
-    <cfRule type="expression" priority="292" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="292" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I43 = "", $A43 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="expression" priority="293" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="293" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $C43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" priority="294" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="294" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $B43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43">
-    <cfRule type="cellIs" priority="295" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="295" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="expression" priority="296" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="296" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G43 = ""), $H43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="containsText" priority="297" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="297" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" priority="298" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="298" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A43="begin group", NOT($B43 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" priority="299" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="299" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A43="end group", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="cellIs" priority="300" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="300" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" priority="301" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="301" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A43="begin repeat", NOT($B43 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" priority="302" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="302" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A43="end repeat", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="expression" priority="303" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="303" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I49 = "", $A49 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="expression" priority="304" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="304" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A49 = "end group"), NOT($A49 = "end repeat"), NOT($A49 = "")), $C49 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="expression" priority="305" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="305" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A49 = "end group"), NOT($A49 = "end repeat"), NOT($A49 = "")), $B49 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="cellIs" priority="306" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="306" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="expression" priority="307" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="307" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G49 = ""), $H49 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="containsText" priority="308" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="308" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="expression" priority="309" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="309" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A49="begin group", NOT($B49 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="expression" priority="310" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="310" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A49="end group", $B49 = "", $C49 = "", $D49 = "", $E49 = "", $F49 = "", $G49 = "", $H49 = "", $I49 = "", $J49 = "", $K49 = "", $L49 = "", $M49 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="cellIs" priority="311" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="311" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="expression" priority="312" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="312" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A49="begin repeat", NOT($B49 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="expression" priority="313" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="313" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A49="end repeat", $B49 = "", $C49 = "", $D49 = "", $E49 = "", $F49 = "", $G49 = "", $H49 = "", $I49 = "", $J49 = "", $K49 = "", $L49 = "", $M49 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:I63">
-    <cfRule type="expression" priority="314" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="314" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I61 = "", $A61 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:C63">
-    <cfRule type="expression" priority="315" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="315" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A61 = "end group"), NOT($A61 = "end repeat"), NOT($A61 = "")), $C61 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61:B63">
-    <cfRule type="expression" priority="316" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="316" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A61 = "end group"), NOT($A61 = "end repeat"), NOT($A61 = "")), $B61 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="cellIs" priority="317" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="317" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H61:H63">
-    <cfRule type="expression" priority="318" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="318" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G61 = ""), $H61 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="containsText" priority="319" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="319" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="expression" priority="320" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="320" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A61="begin group", NOT($B61 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="expression" priority="321" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="321" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A61="end group", $B61 = "", $C61 = "", $D61 = "", $E61 = "", $F61 = "", $G61 = "", $H61 = "", $I61 = "", $J61 = "", $K61 = "", $L61 = "", $M61 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="cellIs" priority="322" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="322" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="expression" priority="323" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="323" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A61="begin repeat", NOT($B61 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="expression" priority="324" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="324" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A61="end repeat", $B61 = "", $C61 = "", $D61 = "", $E61 = "", $F61 = "", $G61 = "", $H61 = "", $I61 = "", $J61 = "", $K61 = "", $L61 = "", $M61 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:Y38">
-    <cfRule type="containsText" priority="325" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="325" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:Y38">
-    <cfRule type="cellIs" priority="326" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="326" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38">
-    <cfRule type="cellIs" priority="327" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="327" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:I48">
-    <cfRule type="expression" priority="328" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="328" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I47 = "", $A47 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="containsText" priority="329" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="329" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="expression" priority="330" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="330" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A85="begin group", NOT($B85 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="expression" priority="331" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="331" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A85="end group", $B85 = "", $C85 = "", $D85 = "", $E85 = "", $F85 = "", $G85 = "", $H85 = "", $I85 = "", $J85 = "", $K85 = "", $L85 = "", $M85 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="cellIs" priority="332" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="332" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="expression" priority="333" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="333" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A85="begin repeat", NOT($B85 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85">
-    <cfRule type="expression" priority="334" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="334" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A85="end repeat", $B85 = "", $C85 = "", $D85 = "", $E85 = "", $F85 = "", $G85 = "", $H85 = "", $I85 = "", $J85 = "", $K85 = "", $L85 = "", $M85 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="containsText" priority="335" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="335" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="expression" priority="336" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="336" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A83="begin group", NOT($B83 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="expression" priority="337" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="337" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A83="end group", $B83 = "", $C83 = "", $D83 = "", $E83 = "", $F83 = "", $G83 = "", $H83 = "", $I83 = "", $J83 = "", $K83 = "", $L83 = "", $M83 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="cellIs" priority="338" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="338" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="expression" priority="339" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="339" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A83 = "end group"), NOT($A83 = "end repeat"), NOT($A83 = "")), $B83 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="expression" priority="340" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="340" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A83="begin repeat", NOT($B83 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="expression" priority="341" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="341" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A83="end repeat", $B83 = "", $C83 = "", $D83 = "", $E83 = "", $F83 = "", $G83 = "", $H83 = "", $I83 = "", $J83 = "", $K83 = "", $L83 = "", $M83 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="containsText" priority="342" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="342" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" priority="343" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="343" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A84="begin group", NOT($B84 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" priority="344" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="344" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A84="end group", $B84 = "", $C84 = "", $D84 = "", $E84 = "", $F84 = "", $G84 = "", $H84 = "", $I84 = "", $J84 = "", $K84 = "", $L84 = "", $M84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="cellIs" priority="345" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="345" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="cellIs" priority="346" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="346" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" priority="347" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="347" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A84="begin repeat", NOT($B84 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A84">
-    <cfRule type="expression" priority="348" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="348" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A84="end repeat", $B84 = "", $C84 = "", $D84 = "", $E84 = "", $F84 = "", $G84 = "", $H84 = "", $I84 = "", $J84 = "", $K84 = "", $L84 = "", $M84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="containsText" priority="349" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="349" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="expression" priority="350" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="350" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A84="begin group", NOT($B84 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="expression" priority="351" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="351" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A84="end group", $B84 = "", $C84 = "", $D84 = "", $E84 = "", $F84 = "", $G84 = "", $H84 = "", $I84 = "", $J84 = "", $K84 = "", $L84 = "", $M84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="cellIs" priority="352" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="352" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="expression" priority="353" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="353" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A84 = "end group"), NOT($A84 = "end repeat"), NOT($A84 = "")), $B84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="expression" priority="354" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="354" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A84="begin repeat", NOT($B84 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84">
-    <cfRule type="expression" priority="355" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="355" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A84="end repeat", $B84 = "", $C84 = "", $D84 = "", $E84 = "", $F84 = "", $G84 = "", $H84 = "", $I84 = "", $J84 = "", $K84 = "", $L84 = "", $M84 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E131">
-    <cfRule type="containsText" priority="356" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="356" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E131">
-    <cfRule type="expression" priority="357" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="357" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A131="begin group", NOT($B131 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E131">
-    <cfRule type="expression" priority="358" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="358" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A131="end group", $B131 = "", $C131 = "", $D131 = "", $E131 = "", $F131 = "", $G131 = "", $H131 = "", $I131 = "", $J131 = "", $K131 = "", $L131 = "", $M131 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E131">
-    <cfRule type="cellIs" priority="359" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="359" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E131">
-    <cfRule type="expression" priority="360" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="360" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A131="begin repeat", NOT($B131 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E131">
-    <cfRule type="expression" priority="361" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="361" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A131="end repeat", $B131 = "", $C131 = "", $D131 = "", $E131 = "", $F131 = "", $G131 = "", $H131 = "", $I131 = "", $J131 = "", $K131 = "", $L131 = "", $M131 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E132">
-    <cfRule type="containsText" priority="362" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="362" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E132">
-    <cfRule type="expression" priority="363" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="363" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A132="begin group", NOT($B132 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E132">
-    <cfRule type="expression" priority="364" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="364" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A132="end group", $B132 = "", $C132 = "", $D132 = "", $E132 = "", $F132 = "", $G132 = "", $H132 = "", $I132 = "", $J132 = "", $K132 = "", $L132 = "", $M132 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E132">
-    <cfRule type="cellIs" priority="365" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="365" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E132">
-    <cfRule type="expression" priority="366" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="366" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A132="begin repeat", NOT($B132 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E132">
-    <cfRule type="expression" priority="367" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="367" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A132="end repeat", $B132 = "", $C132 = "", $D132 = "", $E132 = "", $F132 = "", $G132 = "", $H132 = "", $I132 = "", $J132 = "", $K132 = "", $L132 = "", $M132 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E133">
-    <cfRule type="containsText" priority="368" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="368" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E133">
-    <cfRule type="expression" priority="369" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="369" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A133="begin group", NOT($B133 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E133">
-    <cfRule type="expression" priority="370" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="370" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A133="end group", $B133 = "", $C133 = "", $D133 = "", $E133 = "", $F133 = "", $G133 = "", $H133 = "", $I133 = "", $J133 = "", $K133 = "", $L133 = "", $M133 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E133">
-    <cfRule type="cellIs" priority="371" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="371" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E133">
-    <cfRule type="expression" priority="372" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="372" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A133="begin repeat", NOT($B133 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E133">
-    <cfRule type="expression" priority="373" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="373" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A133="end repeat", $B133 = "", $C133 = "", $D133 = "", $E133 = "", $F133 = "", $G133 = "", $H133 = "", $I133 = "", $J133 = "", $K133 = "", $L133 = "", $M133 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I75">
-    <cfRule type="expression" priority="374" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="374" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I75 = "", $A75 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="expression" priority="375" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="375" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A75 = "end group"), NOT($A75 = "end repeat"), NOT($A75 = "")), $C75 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="expression" priority="376" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="376" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A75 = "end group"), NOT($A75 = "end repeat"), NOT($A75 = "")), $B75 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A75">
-    <cfRule type="cellIs" priority="377" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="377" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75">
-    <cfRule type="expression" priority="378" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="378" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G75 = ""), $H75 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="expression" priority="379" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="379" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I86 = "", $A86 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="expression" priority="380" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="380" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A86 = "end group"), NOT($A86 = "end repeat"), NOT($A86 = "")), $C86 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86">
-    <cfRule type="cellIs" priority="381" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="cellIs" priority="381" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H86">
-    <cfRule type="expression" priority="382" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="382" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G86 = ""), $H86 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="containsText" priority="383" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="56"/>
+    <cfRule type="containsText" priority="383" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="expression" priority="384" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="384" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A86="begin group", NOT($B86 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="expression" priority="385" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
+    <cfRule type="expression" priority="385" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A86="end group", $B86 = "", $C86 = "", $D86 = "", $E86 = "", $F86 = "", $G86 = "", $H86 = "", $I86 = "", $J86 = "", $K86 = "", $L86 = "", $M86 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="cellIs" priority="386" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
+    <cfRule type="cellIs" priority="386" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="expression" priority="387" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
+    <cfRule type="expression" priority="387" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A86="begin repeat", NOT($B86 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86">
-    <cfRule type="expression" priority="388" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
+    <cfRule type="expression" priority="388" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A86="end repeat", $B86 = "", $C86 = "", $D86 = "", $E86 = "", $F86 = "", $G86 = "", $H86 = "", $I86 = "", $J86 = "", $K86 = "", $L86 = "", $M86 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B136">
-    <cfRule type="expression" priority="389" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
+    <cfRule type="expression" priority="389" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>COUNTIF($B$2:$B$1091,B136)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B131">
-    <cfRule type="expression" priority="390" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
+    <cfRule type="expression" priority="390" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>COUNTIF($B$2:$B$1095,B131)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B132">
-    <cfRule type="expression" priority="391" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
+    <cfRule type="expression" priority="391" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>COUNTIF($B$2:$B$1094,B132)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68:B69">
-    <cfRule type="expression" priority="392" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
+    <cfRule type="expression" priority="392" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>COUNTIF($B$2:$B$1083,B68)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B81">
-    <cfRule type="expression" priority="393" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="393" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>COUNTIF($B$2:$B$1074,B80)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" priority="394" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="394" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>COUNTIF($B$2:$B$995,B43)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:B84">
-    <cfRule type="expression" priority="395" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="395" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>COUNTIF($B$2:$B$1096,B83)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:A63">
-    <cfRule type="cellIs" priority="396" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="396" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="containsText" priority="397" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+    <cfRule type="containsText" priority="397" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="expression" priority="398" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="398" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A89="begin group", NOT($B89 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="expression" priority="399" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="399" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A89="end group", $B89 = "", $C89 = "", $D89 = "", $E89 = "", $F89 = "", $G89 = "", $H89 = "", $I89 = "", $J89 = "", $K89 = "", $L89 = "", $M89 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" priority="400" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="400" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="expression" priority="401" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="401" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A89="begin repeat", NOT($B89 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="expression" priority="402" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="402" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A89="end repeat", $B89 = "", $C89 = "", $D89 = "", $E89 = "", $F89 = "", $G89 = "", $H89 = "", $I89 = "", $J89 = "", $K89 = "", $L89 = "", $M89 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:Y37">
-    <cfRule type="containsText" priority="403" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+    <cfRule type="containsText" priority="403" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:Y37">
-    <cfRule type="cellIs" priority="404" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="404" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="cellIs" priority="405" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="405" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="containsText" priority="406" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+    <cfRule type="containsText" priority="406" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="expression" priority="407" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="407" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A14="begin group", NOT($B14 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="expression" priority="408" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="408" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A14="end group", $B14 = "", $C14 = "", $D14 = "", $E14 = "", $F14 = "", $G14 = "", $H14 = "", $I14 = "", $J14 = "", $K14 = "", $L14 = "", $M14 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="cellIs" priority="409" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="409" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="expression" priority="410" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="410" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($I14 = "", $A14 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" priority="411" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="411" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(AND(NOT($A14 = "end group"), NOT($A14 = "end repeat"), NOT($A14 = "")), $C14 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" priority="412" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="412" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(AND(NOT($A14 = "end group"), NOT($A14 = "end repeat"), NOT($A14 = "")), $B14 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" priority="413" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="413" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="expression" priority="414" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="414" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(NOT($G14 = ""), $H14 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="expression" priority="415" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="415" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A14="begin repeat", NOT($B14 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:Y14">
-    <cfRule type="expression" priority="416" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="416" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A14="end repeat", $B14 = "", $C14 = "", $D14 = "", $E14 = "", $F14 = "", $G14 = "", $H14 = "", $I14 = "", $J14 = "", $K14 = "", $L14 = "", $M14 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="expression" priority="417" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="417" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($I42 = "", $A42 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="containsText" priority="418" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+    <cfRule type="containsText" priority="418" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="expression" priority="419" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="419" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A42="begin group", NOT($B42 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="expression" priority="420" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="420" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A42="end group", $B42 = "", $C42 = "", $D42 = "", $E42 = "", $F42 = "", $G42 = "", $H42 = "", $I42 = "", $J42 = "", $K42 = "", $L42 = "", $M42 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" priority="421" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="421" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="expression" priority="422" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="422" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A42="begin repeat", NOT($B42 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42">
-    <cfRule type="expression" priority="423" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="423" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A42="end repeat", $B42 = "", $C42 = "", $D42 = "", $E42 = "", $F42 = "", $G42 = "", $H42 = "", $I42 = "", $J42 = "", $K42 = "", $L42 = "", $M42 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65">
-    <cfRule type="expression" priority="424" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="424" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($I65 = "", $A65 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" priority="425" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="425" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(AND(NOT($A65 = "end group"), NOT($A65 = "end repeat"), NOT($A65 = "")), $C65 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="expression" priority="426" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="426" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(AND(NOT($A65 = "end group"), NOT($A65 = "end repeat"), NOT($A65 = "")), $B65 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="cellIs" priority="427" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="427" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65">
-    <cfRule type="expression" priority="428" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="428" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(NOT($G65 = ""), $H65 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="containsText" priority="429" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+    <cfRule type="containsText" priority="429" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="expression" priority="430" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="430" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A65="begin group", NOT($B65 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="expression" priority="431" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="431" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A65="end group", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" priority="432" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="432" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="expression" priority="433" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="433" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A65="begin repeat", NOT($B65 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="expression" priority="434" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="434" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A65="end repeat", $B65 = "", $C65 = "", $D65 = "", $E65 = "", $F65 = "", $G65 = "", $H65 = "", $I65 = "", $J65 = "", $K65 = "", $L65 = "", $M65 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I66">
-    <cfRule type="expression" priority="435" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="435" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($I66 = "", $A66 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" priority="436" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="436" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $C66 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="expression" priority="437" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="437" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(AND(NOT($A66 = "end group"), NOT($A66 = "end repeat"), NOT($A66 = "")), $B66 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="cellIs" priority="438" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="438" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H66">
-    <cfRule type="expression" priority="439" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="439" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(NOT($G66 = ""), $H66 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="containsText" priority="440" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+    <cfRule type="containsText" priority="440" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="441" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="441" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A66="begin group", NOT($B66 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="442" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="442" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A66="end group", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" priority="443" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="443" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="444" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="444" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A66="begin repeat", NOT($B66 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="expression" priority="445" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="445" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($A66="end repeat", $B66 = "", $C66 = "", $D66 = "", $E66 = "", $F66 = "", $G66 = "", $H66 = "", $I66 = "", $J66 = "", $K66 = "", $L66 = "", $M66 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44">
-    <cfRule type="expression" priority="446" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="446" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND($I44 = "", $A44 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" priority="447" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="447" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $C44 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="expression" priority="448" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="448" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(AND(NOT($A44 = "end group"), NOT($A44 = "end repeat"), NOT($A44 = "")), $B44 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="cellIs" priority="449" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="cellIs" priority="449" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="expression" priority="450" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="450" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>AND(NOT($G44 = ""), $H44 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="containsText" priority="451" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="64"/>
+    <cfRule type="containsText" priority="451" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" priority="452" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="452" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A44="begin group", NOT($B44 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" priority="453" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="453" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A44="end group", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="cellIs" priority="454" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="cellIs" priority="454" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" priority="455" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="455" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A44="begin repeat", NOT($B44 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" priority="456" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="456" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($A44="end repeat", $B44 = "", $C44 = "", $D44 = "", $E44 = "", $F44 = "", $G44 = "", $H44 = "", $I44 = "", $J44 = "", $K44 = "", $L44 = "", $M44 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45">
-    <cfRule type="expression" priority="457" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="457" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND($I45 = "", $A45 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="expression" priority="458" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="458" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $C45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="expression" priority="459" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+    <cfRule type="expression" priority="459" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(AND(NOT($A45 = "end group"), NOT($A45 = "end repeat"), NOT($A45 = "")), $B45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="cellIs" priority="460" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
+    <cfRule type="cellIs" priority="460" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="expression" priority="461" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
+    <cfRule type="expression" priority="461" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>AND(NOT($G45 = ""), $H45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="containsText" priority="462" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="67"/>
+    <cfRule type="containsText" priority="462" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="expression" priority="463" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="463" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A45="begin group", NOT($B45 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="expression" priority="464" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="464" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A45="end group", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="cellIs" priority="465" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="cellIs" priority="465" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="expression" priority="466" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="466" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A45="begin repeat", NOT($B45 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="expression" priority="467" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="467" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($A45="end repeat", $B45 = "", $C45 = "", $D45 = "", $E45 = "", $F45 = "", $G45 = "", $H45 = "", $I45 = "", $J45 = "", $K45 = "", $L45 = "", $M45 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53">
-    <cfRule type="expression" priority="468" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="468" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND($I53 = "", $A53 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="expression" priority="469" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
+    <cfRule type="expression" priority="469" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
       <formula>AND(AND(NOT($A53 = "end group"), NOT($A53 = "end repeat"), NOT($A53 = "")), $C53 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53">
-    <cfRule type="cellIs" priority="470" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="cellIs" priority="470" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="expression" priority="471" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="expression" priority="471" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND(NOT($G53 = ""), $H53 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="containsText" priority="472" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="68"/>
+    <cfRule type="containsText" priority="472" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="expression" priority="473" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="expression" priority="473" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A53="begin group", NOT($B53 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="expression" priority="474" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="expression" priority="474" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A53="end group", $B53 = "", $C53 = "", $D53 = "", $E53 = "", $F53 = "", $G53 = "", $H53 = "", $I53 = "", $J53 = "", $K53 = "", $L53 = "", $M53 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" priority="475" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="cellIs" priority="475" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="expression" priority="476" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="expression" priority="476" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>AND($A53="begin repeat", NOT($B53 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="expression" priority="477" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
+    <cfRule type="expression" priority="477" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>AND($A53="end repeat", $B53 = "", $C53 = "", $D53 = "", $E53 = "", $F53 = "", $G53 = "", $H53 = "", $I53 = "", $J53 = "", $K53 = "", $L53 = "", $M53 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:A55">
-    <cfRule type="cellIs" priority="478" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
+    <cfRule type="cellIs" priority="478" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54:E55">
-    <cfRule type="containsText" priority="479" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="71"/>
+    <cfRule type="containsText" priority="479" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54:E55">
-    <cfRule type="cellIs" priority="480" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
+    <cfRule type="cellIs" priority="480" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="containsText" priority="481" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="73"/>
+    <cfRule type="containsText" priority="481" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:Y55">
-    <cfRule type="cellIs" priority="482" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
+    <cfRule type="cellIs" priority="482" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55">
-    <cfRule type="cellIs" priority="483" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
+    <cfRule type="cellIs" priority="483" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="expression" priority="484" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
+    <cfRule type="expression" priority="484" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>COUNTIF($B$2:$B$994,B49)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="485" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
+    <cfRule type="expression" priority="485" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>AND(A1 = "type", COUNTIF($A$1:$A$1099, "begin group") = COUNTIF($A$1:$A$1099, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="486" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
+    <cfRule type="expression" priority="486" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$1090, "begin group") = COUNTIF($A$1:$A$1099, "end group")))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57">
-    <cfRule type="expression" priority="487" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="487" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($I57 = "", $A57 = "calculate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="expression" priority="488" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="488" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(AND(NOT($A57 = "end group"), NOT($A57 = "end repeat"), NOT($A57 = "")), $C57 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="cellIs" priority="489" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="cellIs" priority="489" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H57">
-    <cfRule type="expression" priority="490" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="490" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND(NOT($G57 = ""), $H57 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="containsText" priority="491" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="50"/>
+    <cfRule type="containsText" priority="491" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="492" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="492" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A57="begin group", NOT($B57 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="493" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="493" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A57="end group", $B57 = "", $C57 = "", $D57 = "", $E57 = "", $F57 = "", $G57 = "", $H57 = "", $I57 = "", $J57 = "", $K57 = "", $L57 = "", $M57 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" priority="494" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="cellIs" priority="494" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="495" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="495" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A57="begin repeat", NOT($B57 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E57">
-    <cfRule type="expression" priority="496" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
+    <cfRule type="expression" priority="496" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>AND($A57="end repeat", $B57 = "", $C57 = "", $D57 = "", $E57 = "", $F57 = "", $G57 = "", $H57 = "", $I57 = "", $J57 = "", $K57 = "", $L57 = "", $M57 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58:E59">
-    <cfRule type="containsText" priority="497" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="14"/>
+    <cfRule type="containsText" priority="497" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58:E59">
-    <cfRule type="expression" priority="498" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="498" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A58="begin group", NOT($B58 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58:E59">
-    <cfRule type="expression" priority="499" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="499" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A58="end group", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58:E59">
-    <cfRule type="cellIs" priority="500" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="cellIs" priority="500" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58:E59">
-    <cfRule type="expression" priority="501" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="501" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A58="begin repeat", NOT($B58 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E58:E59">
-    <cfRule type="expression" priority="502" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="502" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A58="end repeat", $B58 = "", $C58 = "", $D58 = "", $E58 = "", $F58 = "", $G58 = "", $H58 = "", $I58 = "", $J58 = "", $K58 = "", $L58 = "", $M58 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E63">
-    <cfRule type="containsText" priority="503" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="14"/>
+    <cfRule type="containsText" priority="503" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E63">
-    <cfRule type="expression" priority="504" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="504" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A62="begin group", NOT($B62 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E63">
-    <cfRule type="expression" priority="505" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="505" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A62="end group", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E63">
-    <cfRule type="cellIs" priority="506" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="cellIs" priority="506" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E63">
-    <cfRule type="expression" priority="507" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="507" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A62="begin repeat", NOT($B62 = ""))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E63">
-    <cfRule type="expression" priority="508" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+    <cfRule type="expression" priority="508" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>AND($A62="end repeat", $B62 = "", $C62 = "", $D62 = "", $E62 = "", $F62 = "", $G62 = "", $H62 = "", $I62 = "", $J62 = "", $K62 = "", $L62 = "", $M62 = "")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10558,17 +10016,16 @@
   <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B104" activeCellId="0" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="65.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="80.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="102.413265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="72.8979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="89.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="113.841836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11830,43 +11287,43 @@
       <c r="E102" s="13"/>
       <c r="F102" s="13"/>
     </row>
-    <row r="103" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="13" t="s">
         <v>470</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>432</v>
+        <v>471</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>288</v>
+        <v>472</v>
       </c>
       <c r="D103" s="13"/>
       <c r="E103" s="13"/>
       <c r="F103" s="13"/>
     </row>
-    <row r="104" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="13" t="s">
         <v>470</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>433</v>
+        <v>473</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>291</v>
+        <v>474</v>
       </c>
       <c r="D104" s="13"/>
       <c r="E104" s="13"/>
       <c r="F104" s="13"/>
     </row>
-    <row r="105" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="13" t="s">
         <v>470</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>434</v>
+        <v>475</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>294</v>
+        <v>476</v>
       </c>
       <c r="D105" s="13"/>
       <c r="E105" s="13"/>
@@ -11877,24 +11334,24 @@
         <v>470</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="D106" s="13"/>
       <c r="E106" s="13"/>
       <c r="F106" s="13"/>
     </row>
-    <row r="107" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="13" t="s">
         <v>470</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>471</v>
+        <v>435</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>472</v>
+        <v>297</v>
       </c>
       <c r="D107" s="13"/>
       <c r="E107" s="13"/>
@@ -11905,10 +11362,10 @@
         <v>470</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="D108" s="13"/>
       <c r="E108" s="13"/>
@@ -11919,189 +11376,203 @@
         <v>470</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="D109" s="13"/>
       <c r="E109" s="13"/>
       <c r="F109" s="13"/>
     </row>
-    <row r="110" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="13" t="s">
         <v>470</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>436</v>
+        <v>481</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>271</v>
+        <v>482</v>
       </c>
       <c r="D110" s="13"/>
       <c r="E110" s="13"/>
       <c r="F110" s="13"/>
     </row>
-    <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="13" t="s">
-        <v>477</v>
-      </c>
-      <c r="B112" s="13" t="s">
-        <v>424</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="D112" s="13"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
+    <row r="111" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="B111" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
     </row>
     <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="13" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>302</v>
+        <v>262</v>
       </c>
       <c r="D113" s="13"/>
       <c r="E113" s="13"/>
       <c r="F113" s="13"/>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="13" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>478</v>
+        <v>420</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>479</v>
+        <v>302</v>
       </c>
       <c r="D114" s="13"/>
       <c r="E114" s="13"/>
       <c r="F114" s="13"/>
     </row>
-    <row r="115" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="13" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>436</v>
+        <v>484</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>271</v>
+        <v>485</v>
       </c>
       <c r="D115" s="13"/>
       <c r="E115" s="13"/>
       <c r="F115" s="13"/>
     </row>
-    <row r="118" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
-        <v>480</v>
-      </c>
-      <c r="B118" s="30" t="s">
-        <v>481</v>
-      </c>
-      <c r="C118" s="0" t="s">
-        <v>482</v>
-      </c>
+    <row r="116" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="B116" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="13"/>
     </row>
     <row r="119" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="B119" s="30" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C120" s="0" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="122" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="B122" s="30" t="s">
-        <v>488</v>
-      </c>
-      <c r="C122" s="0" t="s">
-        <v>489</v>
+      <c r="B121" s="30" t="s">
+        <v>491</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
-        <v>492</v>
-      </c>
-      <c r="B126" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>338</v>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B124" s="30" t="s">
+        <v>496</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="B127" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="B128" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C127" s="0" t="s">
+      <c r="C128" s="0" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="31" t="s">
-        <v>493</v>
-      </c>
-      <c r="B129" s="13" t="s">
-        <v>494</v>
-      </c>
-      <c r="C129" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="D129" s="13"/>
-      <c r="E129" s="13"/>
-      <c r="F129" s="13"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="31" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="C130" s="13" t="s">
-        <v>496</v>
+        <v>250</v>
       </c>
       <c r="D130" s="13"/>
       <c r="E130" s="13"/>
       <c r="F130" s="13"/>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="31" t="s">
+        <v>499</v>
+      </c>
+      <c r="B131" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>502</v>
+      </c>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="13"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -12130,47 +11601,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.6071428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="C2" s="32" t="n">
         <f aca="true">NOW()</f>
-        <v>44281.3987149428</v>
+        <v>44293.6328580211</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="F2" s="13"/>
     </row>

</xml_diff>

<commit_message>
fix labels and hts workflows
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_initial_test.xlsx
+++ b/config/default/forms/app/hts_initial_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -504,7 +504,7 @@
     <t xml:space="preserve">_1710_clientConsented_99DCT</t>
   </si>
   <si>
-    <t xml:space="preserve">Has client consented?</t>
+    <t xml:space="preserve">Has consent been given?</t>
   </si>
   <si>
     <t xml:space="preserve">select_one test_mode</t>
@@ -1950,7 +1950,16 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
     <dxf>
       <font>
         <name val="Arial"/>
@@ -2050,27 +2059,25 @@
   <dimension ref="A1:AL65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="47.3367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.8877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="164.867346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="134.362244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="113.030612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="257.295918367347"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="85.8571428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="81.0867346938776"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="102.862244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.0459183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.4744897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="170.897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="139.219387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="117.081632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="266.65306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="88.9132653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="83.9642857142857"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="106.551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4395,7 +4402,7 @@
       <c r="X68" s="9"/>
       <c r="Y68" s="9"/>
     </row>
-    <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
         <v>158</v>
       </c>
@@ -10387,18 +10394,17 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B122" activeCellId="0" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="87.0255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="107.005102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="135.801020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="90.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="110.872448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="140.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11954,9 +11960,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="78.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="81.0867346938776"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11988,7 +11992,7 @@
       </c>
       <c r="C2" s="32" t="n">
         <f aca="true">NOW()</f>
-        <v>44335.923136342</v>
+        <v>44338.8078931827</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>525</v>

</xml_diff>